<commit_message>
Most recent nystagmus values
</commit_message>
<xml_diff>
--- a/code/innerEarModel/Cammille_results/nystagmus.xlsx
+++ b/code/innerEarModel/Cammille_results/nystagmus.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cammillego\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ozenc\Documents\MATLAB\projects\mriTOMEAnalysis\code\innerEarModel\Cammille_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3398870-1B30-44E2-9637-DFF1B1160F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67A44E1-C911-4C83-9764-0EA3AAE49548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5990DE97-AE4B-45E7-8E74-46C050867CA2}"/>
+    <workbookView xWindow="1008" yWindow="2016" windowWidth="21192" windowHeight="8964" xr2:uid="{92F14915-5F3D-46F3-991C-B859FFAC9669}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Patient</t>
   </si>
@@ -42,27 +42,63 @@
     <t>run1_x</t>
   </si>
   <si>
+    <t>run1_x_var</t>
+  </si>
+  <si>
     <t>run1_y</t>
   </si>
   <si>
+    <t>run1_y_var</t>
+  </si>
+  <si>
     <t>run2_x</t>
   </si>
   <si>
+    <t>run2_x_var</t>
+  </si>
+  <si>
     <t>run2_y</t>
   </si>
   <si>
+    <t>run2_y_var</t>
+  </si>
+  <si>
     <t>run3_x</t>
   </si>
   <si>
+    <t>run3_x_var</t>
+  </si>
+  <si>
     <t>run3_y</t>
   </si>
   <si>
+    <t>run3_y_var</t>
+  </si>
+  <si>
     <t>run4_x</t>
   </si>
   <si>
+    <t>run4_x_var</t>
+  </si>
+  <si>
     <t>run4_y</t>
   </si>
   <si>
+    <t>run4_y_var</t>
+  </si>
+  <si>
+    <t>Mean X</t>
+  </si>
+  <si>
+    <t>Std X</t>
+  </si>
+  <si>
+    <t>Mean Y</t>
+  </si>
+  <si>
+    <t>Std Y</t>
+  </si>
+  <si>
     <t>TOME_3001</t>
   </si>
   <si>
@@ -90,88 +126,88 @@
     <t>TOME_3014</t>
   </si>
   <si>
+    <t>TOME_3046</t>
+  </si>
+  <si>
+    <t>TOME_3045</t>
+  </si>
+  <si>
+    <t>TOME_3044</t>
+  </si>
+  <si>
+    <t>TOME_3043</t>
+  </si>
+  <si>
+    <t>TOME_3042</t>
+  </si>
+  <si>
+    <t>TOME_3040</t>
+  </si>
+  <si>
+    <t>TOME_3039</t>
+  </si>
+  <si>
+    <t>TOME_3038</t>
+  </si>
+  <si>
+    <t>TOME_3036</t>
+  </si>
+  <si>
+    <t>TOME_3035</t>
+  </si>
+  <si>
+    <t>TOME_3034</t>
+  </si>
+  <si>
+    <t>TOME_3033</t>
+  </si>
+  <si>
+    <t>TOME_3032</t>
+  </si>
+  <si>
+    <t>TOME_3031</t>
+  </si>
+  <si>
+    <t>TOME_3030</t>
+  </si>
+  <si>
+    <t>TOME_3029</t>
+  </si>
+  <si>
+    <t>TOME_3028</t>
+  </si>
+  <si>
+    <t>TOME_3026</t>
+  </si>
+  <si>
+    <t>TOME_3025</t>
+  </si>
+  <si>
+    <t>TOME_3024</t>
+  </si>
+  <si>
+    <t>TOME_3023</t>
+  </si>
+  <si>
+    <t>TOME_3022</t>
+  </si>
+  <si>
+    <t>TOME_3021</t>
+  </si>
+  <si>
+    <t>TOME_3020</t>
+  </si>
+  <si>
+    <t>TOME_3019</t>
+  </si>
+  <si>
+    <t>TOME_3018</t>
+  </si>
+  <si>
+    <t>TOME_3016</t>
+  </si>
+  <si>
     <t>TOME_3015</t>
-  </si>
-  <si>
-    <t>TOME_3016</t>
-  </si>
-  <si>
-    <t>TOME_3018</t>
-  </si>
-  <si>
-    <t>TOME_3019</t>
-  </si>
-  <si>
-    <t>TOME_3020</t>
-  </si>
-  <si>
-    <t>TOME_3021</t>
-  </si>
-  <si>
-    <t>TOME_3022</t>
-  </si>
-  <si>
-    <t>TOME_3023</t>
-  </si>
-  <si>
-    <t>TOME_3024</t>
-  </si>
-  <si>
-    <t>TOME_3025</t>
-  </si>
-  <si>
-    <t>TOME_3026</t>
-  </si>
-  <si>
-    <t>TOME_3028</t>
-  </si>
-  <si>
-    <t>TOME_3029</t>
-  </si>
-  <si>
-    <t>TOME_3030</t>
-  </si>
-  <si>
-    <t>TOME_3031</t>
-  </si>
-  <si>
-    <t>TOME_3032</t>
-  </si>
-  <si>
-    <t>TOME_3033</t>
-  </si>
-  <si>
-    <t>TOME_3034</t>
-  </si>
-  <si>
-    <t>TOME_3035</t>
-  </si>
-  <si>
-    <t>TOME_3036</t>
-  </si>
-  <si>
-    <t>TOME_3038</t>
-  </si>
-  <si>
-    <t>TOME_3039</t>
-  </si>
-  <si>
-    <t>TOME_3040</t>
-  </si>
-  <si>
-    <t>TOME_3042</t>
-  </si>
-  <si>
-    <t>TOME_3043</t>
-  </si>
-  <si>
-    <t>TOME_3044</t>
-  </si>
-  <si>
-    <t>TOME_3045</t>
-  </si>
-  <si>
-    <t>TOME_3046</t>
   </si>
 </sst>
 </file>
@@ -525,19 +561,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B8C0D34-0109-46A3-972F-AA9C0B82FC3F}">
-  <dimension ref="A1:I38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC9FD20F-EF65-4AAB-A490-142DE5A8DA8F}">
+  <dimension ref="A1:U38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -565,1060 +601,2410 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>-0.99938000000000005</v>
       </c>
       <c r="C2">
+        <v>2.3168000000000002</v>
+      </c>
+      <c r="D2">
         <v>-1.0660000000000001</v>
       </c>
-      <c r="D2">
+      <c r="E2">
+        <v>0.28813</v>
+      </c>
+      <c r="F2">
         <v>-0.53244999999999998</v>
       </c>
-      <c r="E2">
+      <c r="G2">
+        <v>9.1925000000000007E-2</v>
+      </c>
+      <c r="H2">
         <v>-1.0004</v>
       </c>
-      <c r="F2">
+      <c r="I2">
+        <v>0.11108999999999999</v>
+      </c>
+      <c r="J2">
         <v>-0.69994000000000001</v>
       </c>
-      <c r="G2">
+      <c r="K2">
+        <v>0.23272000000000001</v>
+      </c>
+      <c r="L2">
         <v>-1.4195</v>
       </c>
-      <c r="H2">
+      <c r="M2">
+        <v>0.89683000000000002</v>
+      </c>
+      <c r="N2">
         <v>-0.76973000000000003</v>
       </c>
-      <c r="I2">
+      <c r="O2">
+        <v>0.18079999999999999</v>
+      </c>
+      <c r="P2">
         <v>-1.0485</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q2">
+        <v>0.22178</v>
+      </c>
+      <c r="R2">
+        <v>-0.75038000000000005</v>
+      </c>
+      <c r="S2">
+        <v>0.19356999999999999</v>
+      </c>
+      <c r="T2">
+        <v>-1.1335999999999999</v>
+      </c>
+      <c r="U2">
+        <v>0.19261</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>-0.48710999999999999</v>
       </c>
       <c r="C3">
+        <v>3.9439000000000002E-2</v>
+      </c>
+      <c r="D3">
         <v>-0.20115</v>
       </c>
-      <c r="D3">
+      <c r="E3">
+        <v>4.4089000000000003E-2</v>
+      </c>
+      <c r="F3">
         <v>-3.1941999999999999</v>
       </c>
-      <c r="E3">
+      <c r="G3">
+        <v>0.11668000000000001</v>
+      </c>
+      <c r="H3">
         <v>-0.81605000000000005</v>
       </c>
-      <c r="F3">
+      <c r="I3">
+        <v>6.9640999999999995E-2</v>
+      </c>
+      <c r="J3">
         <v>-2.5998999999999999</v>
       </c>
-      <c r="G3">
+      <c r="K3">
+        <v>0.38138</v>
+      </c>
+      <c r="L3">
         <v>-1.5385</v>
       </c>
-      <c r="H3">
+      <c r="M3">
+        <v>8.8585999999999998E-2</v>
+      </c>
+      <c r="N3">
         <v>-1.0266</v>
       </c>
-      <c r="I3">
+      <c r="O3">
+        <v>0.12565000000000001</v>
+      </c>
+      <c r="P3">
         <v>-1.7937000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q3">
+        <v>0.17122999999999999</v>
+      </c>
+      <c r="R3">
+        <v>-1.827</v>
+      </c>
+      <c r="S3">
+        <v>1.2784</v>
+      </c>
+      <c r="T3">
+        <v>-1.0873999999999999</v>
+      </c>
+      <c r="U3">
+        <v>0.72143999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>-6.7848000000000006E-2</v>
       </c>
       <c r="C4">
+        <v>0.13974</v>
+      </c>
+      <c r="D4">
         <v>-0.38177</v>
       </c>
-      <c r="D4">
+      <c r="E4">
+        <v>0.15462999999999999</v>
+      </c>
+      <c r="F4">
         <v>-0.19577</v>
       </c>
-      <c r="E4">
+      <c r="G4">
+        <v>0.11222</v>
+      </c>
+      <c r="H4">
         <v>-0.54135999999999995</v>
       </c>
-      <c r="F4">
+      <c r="I4">
+        <v>0.11423999999999999</v>
+      </c>
+      <c r="J4">
         <v>0.23419999999999999</v>
       </c>
-      <c r="G4">
+      <c r="K4">
+        <v>0.17191000000000001</v>
+      </c>
+      <c r="L4">
         <v>-0.49776999999999999</v>
       </c>
-      <c r="H4">
+      <c r="M4">
+        <v>0.1079</v>
+      </c>
+      <c r="N4">
         <v>3.6206000000000002E-2</v>
       </c>
-      <c r="I4">
+      <c r="O4">
+        <v>0.19225</v>
+      </c>
+      <c r="P4">
         <v>-0.62751000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q4">
+        <v>0.16399</v>
+      </c>
+      <c r="R4">
+        <v>1.6969999999999999E-3</v>
+      </c>
+      <c r="S4">
+        <v>0.18173</v>
+      </c>
+      <c r="T4">
+        <v>-0.5121</v>
+      </c>
+      <c r="U4">
+        <v>0.10224999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>-2.2121</v>
       </c>
       <c r="C5">
+        <v>0.11839</v>
+      </c>
+      <c r="D5">
         <v>-1.7542</v>
       </c>
-      <c r="D5">
+      <c r="E5">
+        <v>0.11243</v>
+      </c>
+      <c r="F5">
         <v>-1.9715</v>
       </c>
-      <c r="E5">
+      <c r="G5">
+        <v>0.12145</v>
+      </c>
+      <c r="H5">
         <v>-1.4172</v>
       </c>
-      <c r="F5">
+      <c r="I5">
+        <v>5.6942E-2</v>
+      </c>
+      <c r="J5">
         <v>-2.5935000000000001</v>
       </c>
-      <c r="G5">
+      <c r="K5">
+        <v>8.8150000000000006E-2</v>
+      </c>
+      <c r="L5">
         <v>-1.7000999999999999</v>
       </c>
-      <c r="H5">
+      <c r="M5">
+        <v>0.11846</v>
+      </c>
+      <c r="N5">
         <v>-2.7522000000000002</v>
       </c>
-      <c r="I5">
+      <c r="O5">
+        <v>0.13366</v>
+      </c>
+      <c r="P5">
         <v>-1.7918000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q5">
+        <v>7.8076999999999994E-2</v>
+      </c>
+      <c r="R5">
+        <v>-2.3822999999999999</v>
+      </c>
+      <c r="S5">
+        <v>0.35550999999999999</v>
+      </c>
+      <c r="T5">
+        <v>-1.6657999999999999</v>
+      </c>
+      <c r="U5">
+        <v>0.16997000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>0.30288999999999999</v>
       </c>
       <c r="C6">
+        <v>0.29404000000000002</v>
+      </c>
+      <c r="D6">
         <v>-2.9226999999999999</v>
       </c>
-      <c r="D6">
+      <c r="E6">
+        <v>0.92666000000000004</v>
+      </c>
+      <c r="F6">
         <v>0.12792000000000001</v>
       </c>
-      <c r="E6">
+      <c r="G6">
+        <v>0.60760999999999998</v>
+      </c>
+      <c r="H6">
         <v>-3.5070000000000001</v>
       </c>
-      <c r="F6">
+      <c r="I6">
+        <v>0.88754</v>
+      </c>
+      <c r="J6">
         <v>-0.49686000000000002</v>
       </c>
-      <c r="G6">
+      <c r="K6">
+        <v>0.10294</v>
+      </c>
+      <c r="L6">
         <v>-3.2191999999999998</v>
       </c>
-      <c r="H6">
+      <c r="M6">
+        <v>0.36019000000000001</v>
+      </c>
+      <c r="N6">
         <v>-0.12989000000000001</v>
       </c>
-      <c r="I6">
+      <c r="O6">
+        <v>0.33137</v>
+      </c>
+      <c r="P6">
         <v>-2.9687999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q6">
+        <v>0.34310000000000002</v>
+      </c>
+      <c r="R6">
+        <v>-4.8985000000000001E-2</v>
+      </c>
+      <c r="S6">
+        <v>0.34749000000000002</v>
+      </c>
+      <c r="T6">
+        <v>-3.1543999999999999</v>
+      </c>
+      <c r="U6">
+        <v>0.26873999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B7">
         <v>-1.8925000000000001</v>
       </c>
       <c r="C7">
+        <v>6.1589999999999999E-2</v>
+      </c>
+      <c r="D7">
         <v>1.9838</v>
       </c>
-      <c r="D7">
+      <c r="E7">
+        <v>0.10715</v>
+      </c>
+      <c r="F7">
         <v>-1.7031000000000001</v>
       </c>
-      <c r="E7">
+      <c r="G7">
+        <v>0.27238000000000001</v>
+      </c>
+      <c r="H7">
         <v>1.1586000000000001</v>
       </c>
-      <c r="F7">
+      <c r="I7">
+        <v>0.10167</v>
+      </c>
+      <c r="J7">
         <v>-1.2109000000000001</v>
       </c>
-      <c r="G7">
+      <c r="K7">
+        <v>0.16974</v>
+      </c>
+      <c r="L7">
         <v>0.83179999999999998</v>
       </c>
-      <c r="H7">
+      <c r="M7">
+        <v>0.10750999999999999</v>
+      </c>
+      <c r="N7">
         <v>-2.3645</v>
       </c>
-      <c r="I7">
+      <c r="O7">
+        <v>0.29354999999999998</v>
+      </c>
+      <c r="P7">
         <v>2.6303000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q7">
+        <v>0.20149</v>
+      </c>
+      <c r="R7">
+        <v>-1.7927</v>
+      </c>
+      <c r="S7">
+        <v>0.4773</v>
+      </c>
+      <c r="T7">
+        <v>1.6511</v>
+      </c>
+      <c r="U7">
+        <v>0.81308999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>-0.47337000000000001</v>
       </c>
       <c r="C8">
+        <v>0.28134999999999999</v>
+      </c>
+      <c r="D8">
         <v>-1.0555000000000001</v>
       </c>
-      <c r="D8">
+      <c r="E8">
+        <v>0.27594000000000002</v>
+      </c>
+      <c r="F8">
         <v>-0.11143</v>
       </c>
-      <c r="E8">
+      <c r="G8">
+        <v>0.26552999999999999</v>
+      </c>
+      <c r="H8">
         <v>-1.1366000000000001</v>
       </c>
-      <c r="F8">
+      <c r="I8">
+        <v>0.28271000000000002</v>
+      </c>
+      <c r="J8">
         <v>-0.2228</v>
       </c>
-      <c r="G8">
+      <c r="K8">
+        <v>0.28187000000000001</v>
+      </c>
+      <c r="L8">
         <v>-1.6788000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>0.36209000000000002</v>
+      </c>
+      <c r="R8">
+        <v>-0.26919999999999999</v>
+      </c>
+      <c r="S8">
+        <v>0.18537999999999999</v>
+      </c>
+      <c r="T8">
+        <v>-1.2903</v>
+      </c>
+      <c r="U8">
+        <v>0.33889000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B9">
         <v>-2.9457</v>
       </c>
       <c r="C9">
+        <v>0.15665999999999999</v>
+      </c>
+      <c r="D9">
         <v>-1.6008</v>
       </c>
-      <c r="D9">
+      <c r="E9">
+        <v>0.26840000000000003</v>
+      </c>
+      <c r="F9">
         <v>-2.6646000000000001</v>
       </c>
-      <c r="E9">
+      <c r="G9">
+        <v>0.46422000000000002</v>
+      </c>
+      <c r="H9">
         <v>-0.47198000000000001</v>
       </c>
-      <c r="F9">
+      <c r="I9">
+        <v>0.12961</v>
+      </c>
+      <c r="J9">
         <v>-2.3010000000000002</v>
       </c>
-      <c r="G9">
+      <c r="K9">
+        <v>0.12634000000000001</v>
+      </c>
+      <c r="L9">
         <v>0.65151999999999999</v>
       </c>
-      <c r="H9">
+      <c r="M9">
+        <v>0.21826000000000001</v>
+      </c>
+      <c r="N9">
         <v>-2.9097</v>
       </c>
-      <c r="I9">
+      <c r="O9">
+        <v>0.19589000000000001</v>
+      </c>
+      <c r="P9">
         <v>1.9338</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q9">
+        <v>0.35169</v>
+      </c>
+      <c r="R9">
+        <v>-2.7052999999999998</v>
+      </c>
+      <c r="S9">
+        <v>0.29703000000000002</v>
+      </c>
+      <c r="T9">
+        <v>0.12814</v>
+      </c>
+      <c r="U9">
+        <v>1.5147999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B10">
         <v>-0.55593000000000004</v>
       </c>
       <c r="C10">
+        <v>0.13039000000000001</v>
+      </c>
+      <c r="D10">
         <v>-0.48219000000000001</v>
       </c>
-      <c r="D10">
+      <c r="E10">
+        <v>0.24471000000000001</v>
+      </c>
+      <c r="F10">
         <v>-0.56525000000000003</v>
       </c>
-      <c r="E10">
+      <c r="G10">
+        <v>0.17660000000000001</v>
+      </c>
+      <c r="H10">
         <v>-0.17118</v>
       </c>
-      <c r="F10">
+      <c r="I10">
+        <v>9.6684999999999993E-2</v>
+      </c>
+      <c r="J10">
         <v>-0.20065</v>
       </c>
-      <c r="G10">
+      <c r="K10">
+        <v>8.9346999999999996E-2</v>
+      </c>
+      <c r="L10">
         <v>6.6825999999999997E-2</v>
       </c>
-      <c r="H10">
+      <c r="M10">
+        <v>4.8675999999999997E-2</v>
+      </c>
+      <c r="N10">
         <v>-0.26286999999999999</v>
       </c>
-      <c r="I10">
+      <c r="O10">
+        <v>0.11977</v>
+      </c>
+      <c r="P10">
         <v>-0.10735</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q10">
+        <v>5.5939000000000003E-2</v>
+      </c>
+      <c r="R10">
+        <v>-0.39617000000000002</v>
+      </c>
+      <c r="S10">
+        <v>0.19158</v>
+      </c>
+      <c r="T10">
+        <v>-0.17347000000000001</v>
+      </c>
+      <c r="U10">
+        <v>0.22908000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11">
+        <v>57</v>
+      </c>
+      <c r="F11">
         <v>-2.3130000000000002</v>
       </c>
-      <c r="E11">
+      <c r="G11">
+        <v>1.4973000000000001</v>
+      </c>
+      <c r="H11">
         <v>-3.6429999999999998</v>
       </c>
-      <c r="F11">
+      <c r="I11">
+        <v>0.79003999999999996</v>
+      </c>
+      <c r="J11">
         <v>-0.51714000000000004</v>
       </c>
-      <c r="G11">
+      <c r="K11">
+        <v>0.29074</v>
+      </c>
+      <c r="L11">
         <v>-2.5472999999999999</v>
       </c>
-      <c r="H11">
+      <c r="M11">
+        <v>1.0819000000000001</v>
+      </c>
+      <c r="N11">
         <v>-2.3359000000000001</v>
       </c>
-      <c r="I11">
+      <c r="O11">
+        <v>0.34254000000000001</v>
+      </c>
+      <c r="P11">
         <v>-2.6627000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q11">
+        <v>0.48912</v>
+      </c>
+      <c r="R11">
+        <v>-1.722</v>
+      </c>
+      <c r="S11">
+        <v>1.0435000000000001</v>
+      </c>
+      <c r="T11">
+        <v>-2.9510000000000001</v>
+      </c>
+      <c r="U11">
+        <v>0.60206000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="B12">
         <v>-1.5018</v>
       </c>
       <c r="C12">
+        <v>0.73192999999999997</v>
+      </c>
+      <c r="D12">
         <v>-3.5859999999999999</v>
       </c>
-      <c r="D12">
+      <c r="E12">
+        <v>1.1814</v>
+      </c>
+      <c r="F12">
         <v>-1.6613</v>
       </c>
-      <c r="E12">
+      <c r="G12">
+        <v>0.28355000000000002</v>
+      </c>
+      <c r="H12">
         <v>-0.99048999999999998</v>
       </c>
-      <c r="F12">
+      <c r="I12">
+        <v>0.40242</v>
+      </c>
+      <c r="J12">
         <v>-1.6809000000000001</v>
       </c>
-      <c r="G12">
+      <c r="K12">
+        <v>1.4552</v>
+      </c>
+      <c r="L12">
         <v>-0.47426000000000001</v>
       </c>
-      <c r="H12">
+      <c r="M12">
+        <v>0.44002000000000002</v>
+      </c>
+      <c r="N12">
         <v>-1.3701000000000001</v>
       </c>
-      <c r="I12">
+      <c r="O12">
+        <v>0.87365999999999999</v>
+      </c>
+      <c r="P12">
         <v>-4.9183999999999999E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q12">
+        <v>0.72860999999999998</v>
+      </c>
+      <c r="R12">
+        <v>-1.5535000000000001</v>
+      </c>
+      <c r="S12">
+        <v>0.14624000000000001</v>
+      </c>
+      <c r="T12">
+        <v>-1.2749999999999999</v>
+      </c>
+      <c r="U12">
+        <v>1.5880000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="B13">
         <v>-2.0605000000000002</v>
       </c>
       <c r="C13">
+        <v>0.42821999999999999</v>
+      </c>
+      <c r="D13">
         <v>-1.0178</v>
       </c>
-      <c r="D13">
+      <c r="E13">
+        <v>0.18903</v>
+      </c>
+      <c r="F13">
         <v>-1.5589999999999999</v>
       </c>
-      <c r="E13">
+      <c r="G13">
+        <v>0.42591000000000001</v>
+      </c>
+      <c r="H13">
         <v>-1.0834999999999999</v>
       </c>
-      <c r="F13">
+      <c r="I13">
+        <v>0.16464999999999999</v>
+      </c>
+      <c r="J13">
         <v>-1.7251000000000001</v>
       </c>
-      <c r="G13">
+      <c r="K13">
+        <v>0.49223</v>
+      </c>
+      <c r="L13">
         <v>-1.0871999999999999</v>
       </c>
-      <c r="H13">
+      <c r="M13">
+        <v>0.27372000000000002</v>
+      </c>
+      <c r="N13">
         <v>-1.0301</v>
       </c>
-      <c r="I13">
+      <c r="O13">
+        <v>0.43935000000000002</v>
+      </c>
+      <c r="P13">
         <v>-1.5911</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q13">
+        <v>0.19349</v>
+      </c>
+      <c r="R13">
+        <v>-1.5936999999999999</v>
+      </c>
+      <c r="S13">
+        <v>0.42974000000000001</v>
+      </c>
+      <c r="T13">
+        <v>-1.1949000000000001</v>
+      </c>
+      <c r="U13">
+        <v>0.26605000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B14">
         <v>-2.1671999999999998</v>
       </c>
       <c r="C14">
+        <v>1.7698</v>
+      </c>
+      <c r="D14">
         <v>-6.8944000000000005E-2</v>
       </c>
-      <c r="D14">
+      <c r="E14">
+        <v>0.19814000000000001</v>
+      </c>
+      <c r="F14">
         <v>-1.9972000000000001</v>
       </c>
-      <c r="E14">
+      <c r="G14">
+        <v>0.21104000000000001</v>
+      </c>
+      <c r="H14">
         <v>-1.2474000000000001</v>
       </c>
-      <c r="F14">
+      <c r="I14">
+        <v>0.22072</v>
+      </c>
+      <c r="J14">
         <v>-2.2044000000000001</v>
       </c>
-      <c r="G14">
+      <c r="K14">
+        <v>0.10309</v>
+      </c>
+      <c r="L14">
         <v>-1.5755999999999999</v>
       </c>
-      <c r="H14">
+      <c r="M14">
+        <v>0.10881</v>
+      </c>
+      <c r="N14">
         <v>-1.7601</v>
       </c>
-      <c r="I14">
+      <c r="O14">
+        <v>8.8898000000000005E-2</v>
+      </c>
+      <c r="P14">
         <v>-1.1406000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q14">
+        <v>0.11626</v>
+      </c>
+      <c r="R14">
+        <v>-2.0322</v>
+      </c>
+      <c r="S14">
+        <v>0.2026</v>
+      </c>
+      <c r="T14">
+        <v>-1.0081</v>
+      </c>
+      <c r="U14">
+        <v>0.65290999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="B15">
         <v>-0.55783000000000005</v>
       </c>
       <c r="C15">
+        <v>0.25922000000000001</v>
+      </c>
+      <c r="D15">
         <v>-2.5491999999999999</v>
       </c>
-      <c r="D15">
+      <c r="E15">
+        <v>0.50412999999999997</v>
+      </c>
+      <c r="F15">
         <v>-0.81608000000000003</v>
       </c>
-      <c r="E15">
+      <c r="G15">
+        <v>0.26577000000000001</v>
+      </c>
+      <c r="H15">
         <v>-0.54312000000000005</v>
       </c>
-      <c r="F15">
+      <c r="I15">
+        <v>0.32150000000000001</v>
+      </c>
+      <c r="J15">
         <v>-0.31108999999999998</v>
       </c>
-      <c r="G15">
+      <c r="K15">
+        <v>0.26296999999999998</v>
+      </c>
+      <c r="L15">
         <v>-4.6453000000000001E-2</v>
       </c>
-      <c r="H15">
+      <c r="M15">
+        <v>0.23698</v>
+      </c>
+      <c r="N15">
         <v>-0.91190000000000004</v>
       </c>
-      <c r="I15">
+      <c r="O15">
+        <v>0.41619</v>
+      </c>
+      <c r="P15">
         <v>-0.18426999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q15">
+        <v>0.42942999999999998</v>
+      </c>
+      <c r="R15">
+        <v>-0.64922999999999997</v>
+      </c>
+      <c r="S15">
+        <v>0.27050999999999997</v>
+      </c>
+      <c r="T15">
+        <v>-0.83076000000000005</v>
+      </c>
+      <c r="U15">
+        <v>1.1646000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B16">
         <v>-0.62739999999999996</v>
       </c>
       <c r="C16">
+        <v>0.25569999999999998</v>
+      </c>
+      <c r="D16">
         <v>-2.2492000000000001</v>
       </c>
-      <c r="D16">
+      <c r="E16">
+        <v>0.1925</v>
+      </c>
+      <c r="F16">
         <v>-0.76375999999999999</v>
       </c>
-      <c r="E16">
+      <c r="G16">
+        <v>0.63902000000000003</v>
+      </c>
+      <c r="H16">
         <v>-1.4234</v>
       </c>
-      <c r="F16">
+      <c r="I16">
+        <v>0.71292999999999995</v>
+      </c>
+      <c r="J16">
         <v>-0.89681999999999995</v>
       </c>
-      <c r="G16">
+      <c r="K16">
+        <v>0.13777</v>
+      </c>
+      <c r="L16">
         <v>-1.0488</v>
       </c>
-      <c r="H16">
+      <c r="M16">
+        <v>0.24182999999999999</v>
+      </c>
+      <c r="N16">
         <v>-0.88182000000000005</v>
       </c>
-      <c r="I16">
+      <c r="O16">
+        <v>0.22509000000000001</v>
+      </c>
+      <c r="P16">
         <v>-1.4871000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q16">
+        <v>0.48748999999999998</v>
+      </c>
+      <c r="R16">
+        <v>-0.79244999999999999</v>
+      </c>
+      <c r="S16">
+        <v>0.12509000000000001</v>
+      </c>
+      <c r="T16">
+        <v>-1.5521</v>
+      </c>
+      <c r="U16">
+        <v>0.50334000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="B17">
         <v>-4.0850999999999997</v>
       </c>
       <c r="C17">
+        <v>2.1755</v>
+      </c>
+      <c r="D17">
         <v>2.1269</v>
       </c>
-      <c r="D17">
+      <c r="E17">
+        <v>3.3368000000000002</v>
+      </c>
+      <c r="F17">
         <v>-4.0529999999999999</v>
       </c>
-      <c r="E17">
+      <c r="G17">
+        <v>1.1696</v>
+      </c>
+      <c r="H17">
         <v>1.6233</v>
       </c>
-      <c r="H17">
+      <c r="I17">
+        <v>3.6987000000000001</v>
+      </c>
+      <c r="N17">
         <v>-7.9622299999999999</v>
       </c>
-      <c r="I17">
+      <c r="O17">
+        <v>15.5657</v>
+      </c>
+      <c r="P17">
         <v>2.6303999999999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q17">
+        <v>2.5928200000000001</v>
+      </c>
+      <c r="R17">
+        <v>-5.3667999999999996</v>
+      </c>
+      <c r="S17">
+        <v>2.2477999999999998</v>
+      </c>
+      <c r="T17">
+        <v>2.1269</v>
+      </c>
+      <c r="U17">
+        <v>0.50355000000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="B18">
         <v>-1.0356000000000001</v>
       </c>
       <c r="C18">
+        <v>0.81306999999999996</v>
+      </c>
+      <c r="D18">
         <v>0.79029000000000005</v>
       </c>
-      <c r="D18">
+      <c r="E18">
+        <v>0.39193</v>
+      </c>
+      <c r="F18">
         <v>0.20052</v>
       </c>
-      <c r="E18">
+      <c r="G18">
+        <v>0.65769999999999995</v>
+      </c>
+      <c r="H18">
         <v>0.57655000000000001</v>
       </c>
-      <c r="F18">
+      <c r="I18">
+        <v>0.35782999999999998</v>
+      </c>
+      <c r="J18">
         <v>-0.23895</v>
       </c>
-      <c r="G18">
+      <c r="K18">
+        <v>0.40144999999999997</v>
+      </c>
+      <c r="L18">
         <v>-0.23505000000000001</v>
       </c>
-      <c r="H18">
+      <c r="M18">
+        <v>0.20377000000000001</v>
+      </c>
+      <c r="N18">
         <v>-0.47578999999999999</v>
       </c>
-      <c r="I18">
+      <c r="O18">
+        <v>0.33173000000000002</v>
+      </c>
+      <c r="P18">
         <v>-6.5236000000000002E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q18">
+        <v>0.35691000000000001</v>
+      </c>
+      <c r="R18">
+        <v>-0.38745000000000002</v>
+      </c>
+      <c r="S18">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="T18">
+        <v>0.26663999999999999</v>
+      </c>
+      <c r="U18">
+        <v>0.49398999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B19">
         <v>-1.9282999999999999</v>
       </c>
       <c r="C19">
+        <v>0.22672</v>
+      </c>
+      <c r="D19">
         <v>-2.1107</v>
       </c>
-      <c r="D19">
+      <c r="E19">
+        <v>0.17474999999999999</v>
+      </c>
+      <c r="F19">
         <v>-2.8195000000000001</v>
       </c>
-      <c r="E19">
+      <c r="G19">
+        <v>0.50334000000000001</v>
+      </c>
+      <c r="H19">
         <v>-3.1596000000000002</v>
       </c>
-      <c r="F19">
+      <c r="I19">
+        <v>0.83174000000000003</v>
+      </c>
+      <c r="J19">
         <v>-2.6000999999999999</v>
       </c>
-      <c r="G19">
+      <c r="K19">
+        <v>0.54354000000000002</v>
+      </c>
+      <c r="L19">
         <v>-2.4662000000000002</v>
       </c>
-      <c r="H19">
+      <c r="M19">
+        <v>0.67706999999999995</v>
+      </c>
+      <c r="N19">
         <v>-1.5407</v>
       </c>
-      <c r="I19">
+      <c r="O19">
+        <v>0.48009000000000002</v>
+      </c>
+      <c r="P19">
         <v>-2.2118000000000002</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q19">
+        <v>0.70933000000000002</v>
+      </c>
+      <c r="R19">
+        <v>-2.2221000000000002</v>
+      </c>
+      <c r="S19">
+        <v>0.59172000000000002</v>
+      </c>
+      <c r="T19">
+        <v>-2.4870999999999999</v>
+      </c>
+      <c r="U19">
+        <v>0.47264</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="B20">
         <v>-4.9344000000000001</v>
       </c>
       <c r="C20">
+        <v>0.46937000000000001</v>
+      </c>
+      <c r="D20">
         <v>-4.3940000000000001</v>
       </c>
-      <c r="D20">
+      <c r="E20">
+        <v>1.5766</v>
+      </c>
+      <c r="F20">
         <v>-3.8469000000000002</v>
       </c>
-      <c r="E20">
+      <c r="G20">
+        <v>0.36591000000000001</v>
+      </c>
+      <c r="H20">
         <v>-2.9491999999999998</v>
       </c>
-      <c r="F20">
+      <c r="I20">
+        <v>0.39835999999999999</v>
+      </c>
+      <c r="J20">
         <v>-4.9782000000000002</v>
       </c>
-      <c r="G20">
+      <c r="K20">
+        <v>0.51602999999999999</v>
+      </c>
+      <c r="L20">
         <v>-2.9826000000000001</v>
       </c>
-      <c r="H20">
+      <c r="M20">
+        <v>2.0257999999999998</v>
+      </c>
+      <c r="N20">
         <v>-4.7112999999999996</v>
       </c>
-      <c r="I20">
+      <c r="O20">
+        <v>0.54491999999999996</v>
+      </c>
+      <c r="P20">
         <v>-3.2360000000000002</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q20">
+        <v>0.40560000000000002</v>
+      </c>
+      <c r="R20">
+        <v>-4.6177000000000001</v>
+      </c>
+      <c r="S20">
+        <v>0.52698999999999996</v>
+      </c>
+      <c r="T20">
+        <v>-3.3904000000000001</v>
+      </c>
+      <c r="U20">
+        <v>0.68118000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="B21">
         <v>-1.7824</v>
       </c>
       <c r="C21">
+        <v>0.25107000000000002</v>
+      </c>
+      <c r="D21">
         <v>-1.0283</v>
       </c>
-      <c r="D21">
+      <c r="E21">
+        <v>0.45915</v>
+      </c>
+      <c r="F21">
         <v>-1.6475</v>
       </c>
-      <c r="E21">
+      <c r="G21">
+        <v>0.15128</v>
+      </c>
+      <c r="H21">
         <v>-0.14645</v>
       </c>
-      <c r="F21">
+      <c r="I21">
+        <v>0.14283999999999999</v>
+      </c>
+      <c r="J21">
         <v>-2.1257000000000001</v>
       </c>
-      <c r="G21">
+      <c r="K21">
+        <v>0.34046999999999999</v>
+      </c>
+      <c r="L21">
         <v>0.17913999999999999</v>
       </c>
-      <c r="H21">
+      <c r="M21">
+        <v>0.24085000000000001</v>
+      </c>
+      <c r="N21">
         <v>-1.9381999999999999</v>
       </c>
-      <c r="I21">
+      <c r="O21">
+        <v>0.37544</v>
+      </c>
+      <c r="P21">
         <v>0.94521999999999995</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q21">
+        <v>0.24156</v>
+      </c>
+      <c r="R21">
+        <v>-1.8734999999999999</v>
+      </c>
+      <c r="S21">
+        <v>0.20588999999999999</v>
+      </c>
+      <c r="T21">
+        <v>-1.2598E-2</v>
+      </c>
+      <c r="U21">
+        <v>0.81725999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B22">
         <v>-2.5320999999999998</v>
       </c>
       <c r="C22">
+        <v>1.2707999999999999</v>
+      </c>
+      <c r="D22">
         <v>-2.2162000000000002</v>
       </c>
-      <c r="D22">
+      <c r="E22">
+        <v>1.0122</v>
+      </c>
+      <c r="F22">
         <v>-1.3768</v>
       </c>
-      <c r="E22">
+      <c r="G22">
+        <v>1.0667</v>
+      </c>
+      <c r="H22">
         <v>-1.4100999999999999</v>
       </c>
-      <c r="F22">
+      <c r="I22">
+        <v>0.57476000000000005</v>
+      </c>
+      <c r="J22">
         <v>-0.79893000000000003</v>
       </c>
-      <c r="G22">
+      <c r="K22">
+        <v>0.56705000000000005</v>
+      </c>
+      <c r="L22">
         <v>-0.9274</v>
       </c>
-      <c r="H22">
+      <c r="M22">
+        <v>0.12545000000000001</v>
+      </c>
+      <c r="N22">
         <v>-0.95860000000000001</v>
       </c>
-      <c r="I22">
+      <c r="O22">
+        <v>0.41345999999999999</v>
+      </c>
+      <c r="P22">
         <v>-1.0066999999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q22">
+        <v>0.11262</v>
+      </c>
+      <c r="R22">
+        <v>-1.4166000000000001</v>
+      </c>
+      <c r="S22">
+        <v>0.78256000000000003</v>
+      </c>
+      <c r="T22">
+        <v>-1.3900999999999999</v>
+      </c>
+      <c r="U22">
+        <v>0.58989000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="B23">
         <v>0.12497999999999999</v>
       </c>
       <c r="C23">
+        <v>0.12494</v>
+      </c>
+      <c r="D23">
         <v>0.67774000000000001</v>
       </c>
-      <c r="D23">
+      <c r="E23">
+        <v>0.25213000000000002</v>
+      </c>
+      <c r="F23">
         <v>-0.42033999999999999</v>
       </c>
-      <c r="E23">
+      <c r="G23">
+        <v>0.13524</v>
+      </c>
+      <c r="H23">
         <v>1.6741999999999999</v>
       </c>
-      <c r="F23">
+      <c r="I23">
+        <v>0.10977000000000001</v>
+      </c>
+      <c r="J23">
         <v>-0.29470000000000002</v>
       </c>
-      <c r="G23">
+      <c r="K23">
+        <v>0.21631</v>
+      </c>
+      <c r="L23">
         <v>0.83299999999999996</v>
       </c>
-      <c r="H23">
+      <c r="M23">
+        <v>0.31791000000000003</v>
+      </c>
+      <c r="N23">
         <v>0.14399000000000001</v>
       </c>
-      <c r="I23">
+      <c r="O23">
+        <v>0.59004000000000001</v>
+      </c>
+      <c r="P23">
         <v>0.46701999999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q23">
+        <v>0.31670999999999999</v>
+      </c>
+      <c r="R23">
+        <v>-0.11151999999999999</v>
+      </c>
+      <c r="S23">
+        <v>0.28876000000000002</v>
+      </c>
+      <c r="T23">
+        <v>0.91298999999999997</v>
+      </c>
+      <c r="U23">
+        <v>0.52917000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B24">
         <v>-2.4304999999999999</v>
       </c>
       <c r="C24">
+        <v>1.0354000000000001</v>
+      </c>
+      <c r="D24">
         <v>2.4278</v>
       </c>
-      <c r="D24">
+      <c r="E24">
+        <v>1.0986</v>
+      </c>
+      <c r="F24">
         <v>-2.0897000000000001</v>
       </c>
-      <c r="E24">
+      <c r="G24">
+        <v>1.0983000000000001</v>
+      </c>
+      <c r="H24">
         <v>1.0620000000000001</v>
       </c>
-      <c r="F24">
+      <c r="I24">
+        <v>0.94869000000000003</v>
+      </c>
+      <c r="J24">
         <v>-1.5886</v>
       </c>
-      <c r="G24">
+      <c r="K24">
+        <v>0.74746000000000001</v>
+      </c>
+      <c r="L24">
         <v>-0.85265999999999997</v>
       </c>
-      <c r="H24">
+      <c r="M24">
+        <v>0.66578999999999999</v>
+      </c>
+      <c r="N24">
         <v>-2.1745000000000001</v>
       </c>
-      <c r="I24">
+      <c r="O24">
+        <v>0.73746</v>
+      </c>
+      <c r="P24">
         <v>0.60079000000000005</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q24">
+        <v>0.78502000000000005</v>
+      </c>
+      <c r="R24">
+        <v>-2.0708000000000002</v>
+      </c>
+      <c r="S24">
+        <v>0.35260999999999998</v>
+      </c>
+      <c r="T24">
+        <v>0.80947999999999998</v>
+      </c>
+      <c r="U24">
+        <v>1.3527</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B25">
         <v>-0.93359000000000003</v>
       </c>
       <c r="C25">
+        <v>0.71279999999999999</v>
+      </c>
+      <c r="D25">
         <v>-1.1351</v>
       </c>
-      <c r="D25">
+      <c r="E25">
+        <v>0.85775999999999997</v>
+      </c>
+      <c r="F25">
         <v>-2.1882000000000001</v>
       </c>
-      <c r="E25">
+      <c r="G25">
+        <v>0.99572000000000005</v>
+      </c>
+      <c r="H25">
         <v>-2.0181</v>
       </c>
-      <c r="F25">
+      <c r="I25">
+        <v>0.90571000000000002</v>
+      </c>
+      <c r="J25">
         <v>-1.8191999999999999</v>
       </c>
-      <c r="G25">
+      <c r="K25">
+        <v>0.79103000000000001</v>
+      </c>
+      <c r="L25">
         <v>-2.9617</v>
       </c>
-      <c r="H25">
+      <c r="M25">
+        <v>1.0404</v>
+      </c>
+      <c r="N25">
         <v>0.36986000000000002</v>
       </c>
-      <c r="I25">
+      <c r="O25">
+        <v>0.49852999999999997</v>
+      </c>
+      <c r="P25">
         <v>-2.7867999999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q25">
+        <v>1.9656</v>
+      </c>
+      <c r="R25">
+        <v>-1.1428</v>
+      </c>
+      <c r="S25">
+        <v>1.1375999999999999</v>
+      </c>
+      <c r="T25">
+        <v>-2.2254</v>
+      </c>
+      <c r="U25">
+        <v>0.83447000000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B26">
         <v>-2.7178</v>
       </c>
       <c r="C26">
+        <v>0.15146000000000001</v>
+      </c>
+      <c r="D26">
         <v>0.71243999999999996</v>
       </c>
-      <c r="D26">
+      <c r="E26">
+        <v>0.15781000000000001</v>
+      </c>
+      <c r="F26">
         <v>-2.5516999999999999</v>
       </c>
-      <c r="E26">
+      <c r="G26">
+        <v>0.19525000000000001</v>
+      </c>
+      <c r="H26">
         <v>0.84960000000000002</v>
       </c>
-      <c r="F26">
+      <c r="I26">
+        <v>0.13142999999999999</v>
+      </c>
+      <c r="J26">
         <v>-3.3262</v>
       </c>
-      <c r="G26">
+      <c r="K26">
+        <v>0.27242</v>
+      </c>
+      <c r="L26">
         <v>1.2541</v>
       </c>
-      <c r="H26">
+      <c r="M26">
+        <v>0.433</v>
+      </c>
+      <c r="N26">
         <v>-2.6726000000000001</v>
       </c>
-      <c r="I26">
+      <c r="O26">
+        <v>0.15343000000000001</v>
+      </c>
+      <c r="P26">
         <v>1.3366</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q26">
+        <v>0.15701000000000001</v>
+      </c>
+      <c r="R26">
+        <v>-2.8170999999999999</v>
+      </c>
+      <c r="S26">
+        <v>0.34658</v>
+      </c>
+      <c r="T26">
+        <v>1.0382</v>
+      </c>
+      <c r="U26">
+        <v>0.30404999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B27">
         <v>-0.14929999999999999</v>
       </c>
       <c r="C27">
+        <v>0.74444999999999995</v>
+      </c>
+      <c r="D27">
         <v>-1.4670000000000001</v>
       </c>
-      <c r="D27">
+      <c r="E27">
+        <v>1.1109</v>
+      </c>
+      <c r="F27">
         <v>0.15645999999999999</v>
       </c>
-      <c r="E27">
+      <c r="G27">
+        <v>0.57647000000000004</v>
+      </c>
+      <c r="H27">
         <v>-2.2959000000000001</v>
       </c>
-      <c r="F27">
+      <c r="I27">
+        <v>1.4556</v>
+      </c>
+      <c r="J27">
         <v>-1.3781000000000001</v>
       </c>
-      <c r="G27">
+      <c r="K27">
+        <v>0.78876000000000002</v>
+      </c>
+      <c r="L27">
         <v>-1.2716000000000001</v>
       </c>
-      <c r="H27">
+      <c r="M27">
+        <v>1.1834</v>
+      </c>
+      <c r="N27">
         <v>-3.6606000000000001</v>
       </c>
-      <c r="I27">
+      <c r="O27">
+        <v>3.4070999999999998</v>
+      </c>
+      <c r="P27">
         <v>-0.32105</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q27">
+        <v>1.1893</v>
+      </c>
+      <c r="R27">
+        <v>-1.2579</v>
+      </c>
+      <c r="S27">
+        <v>1.7337</v>
+      </c>
+      <c r="T27">
+        <v>-1.3389</v>
+      </c>
+      <c r="U27">
+        <v>0.81093000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B28">
         <v>-5.944E-2</v>
       </c>
       <c r="C28">
+        <v>6.7502000000000006E-2</v>
+      </c>
+      <c r="D28">
         <v>0.24271000000000001</v>
       </c>
-      <c r="D28">
+      <c r="E28">
+        <v>9.4544000000000003E-2</v>
+      </c>
+      <c r="F28">
         <v>4.5878000000000002E-2</v>
       </c>
-      <c r="E28">
+      <c r="G28">
+        <v>6.8199999999999997E-2</v>
+      </c>
+      <c r="H28">
         <v>0.23211999999999999</v>
       </c>
-      <c r="F28">
+      <c r="I28">
+        <v>0.10442</v>
+      </c>
+      <c r="J28">
         <v>0.27736</v>
       </c>
-      <c r="G28">
+      <c r="K28">
+        <v>8.7325E-2</v>
+      </c>
+      <c r="L28">
         <v>0.60402999999999996</v>
       </c>
-      <c r="H28">
+      <c r="M28">
+        <v>0.11860999999999999</v>
+      </c>
+      <c r="N28">
         <v>-0.15823000000000001</v>
       </c>
-      <c r="I28">
+      <c r="O28">
+        <v>9.2101000000000002E-2</v>
+      </c>
+      <c r="P28">
         <v>0.64317000000000002</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q28">
+        <v>0.10588</v>
+      </c>
+      <c r="R28">
+        <v>2.6391999999999999E-2</v>
+      </c>
+      <c r="S28">
+        <v>0.18692</v>
+      </c>
+      <c r="T28">
+        <v>0.43051</v>
+      </c>
+      <c r="U28">
+        <v>0.22358</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B29">
         <v>-1.9359</v>
       </c>
       <c r="C29">
+        <v>0.14715</v>
+      </c>
+      <c r="D29">
         <v>-0.51805999999999996</v>
       </c>
-      <c r="D29">
+      <c r="E29">
+        <v>0.12139</v>
+      </c>
+      <c r="F29">
         <v>-1.6758</v>
       </c>
-      <c r="E29">
+      <c r="G29">
+        <v>0.19613</v>
+      </c>
+      <c r="H29">
         <v>-0.48963000000000001</v>
       </c>
-      <c r="F29">
+      <c r="I29">
+        <v>0.10673000000000001</v>
+      </c>
+      <c r="J29">
         <v>-0.78827000000000003</v>
       </c>
-      <c r="G29">
+      <c r="K29">
+        <v>0.12722</v>
+      </c>
+      <c r="L29">
         <v>-0.47239999999999999</v>
       </c>
-      <c r="H29">
+      <c r="M29">
+        <v>7.9819000000000001E-2</v>
+      </c>
+      <c r="N29">
         <v>-1.1535</v>
       </c>
-      <c r="I29">
+      <c r="O29">
+        <v>0.13879</v>
+      </c>
+      <c r="P29">
         <v>-9.0920000000000001E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q29">
+        <v>6.3678999999999999E-2</v>
+      </c>
+      <c r="R29">
+        <v>-1.3884000000000001</v>
+      </c>
+      <c r="S29">
+        <v>0.51565000000000005</v>
+      </c>
+      <c r="T29">
+        <v>-0.39274999999999999</v>
+      </c>
+      <c r="U29">
+        <v>0.2021</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B30">
         <v>-1.2765</v>
       </c>
       <c r="C30">
+        <v>3.1803999999999999E-2</v>
+      </c>
+      <c r="D30">
         <v>-7.8245999999999996E-2</v>
       </c>
-      <c r="D30">
+      <c r="E30">
+        <v>3.4352000000000001E-2</v>
+      </c>
+      <c r="F30">
         <v>-2.0223</v>
       </c>
-      <c r="E30">
+      <c r="G30">
+        <v>4.7349000000000002E-2</v>
+      </c>
+      <c r="H30">
         <v>-9.5302999999999999E-2</v>
       </c>
-      <c r="F30">
+      <c r="I30">
+        <v>1.9540999999999999E-2</v>
+      </c>
+      <c r="J30">
         <v>-1.4074</v>
       </c>
-      <c r="G30">
+      <c r="K30">
+        <v>9.5160999999999996E-2</v>
+      </c>
+      <c r="L30">
         <v>-0.36009999999999998</v>
       </c>
-      <c r="H30">
+      <c r="M30">
+        <v>5.7789E-2</v>
+      </c>
+      <c r="N30">
         <v>-1.5649999999999999</v>
       </c>
-      <c r="I30">
+      <c r="O30">
+        <v>0.18076999999999999</v>
+      </c>
+      <c r="P30">
         <v>-0.27383000000000002</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q30">
+        <v>5.6208000000000001E-2</v>
+      </c>
+      <c r="R30">
+        <v>-1.5678000000000001</v>
+      </c>
+      <c r="S30">
+        <v>0.32514999999999999</v>
+      </c>
+      <c r="T30">
+        <v>-0.20186999999999999</v>
+      </c>
+      <c r="U30">
+        <v>0.13766</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31">
         <v>-0.71909999999999996</v>
       </c>
       <c r="C31">
+        <v>6.2474000000000002E-2</v>
+      </c>
+      <c r="D31">
         <v>-1.4169</v>
       </c>
-      <c r="D31">
+      <c r="E31">
+        <v>0.32301999999999997</v>
+      </c>
+      <c r="F31">
         <v>8.2199999999999995E-2</v>
       </c>
-      <c r="E31">
+      <c r="G31">
+        <v>5.3213000000000003E-2</v>
+      </c>
+      <c r="H31">
         <v>-1.9015</v>
       </c>
-      <c r="F31">
+      <c r="I31">
+        <v>0.13958999999999999</v>
+      </c>
+      <c r="J31">
         <v>-0.4793</v>
       </c>
-      <c r="G31">
+      <c r="K31">
+        <v>0.18878</v>
+      </c>
+      <c r="L31">
         <v>-1.2794000000000001</v>
       </c>
-      <c r="H31">
+      <c r="M31">
+        <v>0.12584000000000001</v>
+      </c>
+      <c r="N31">
         <v>-0.45762999999999998</v>
       </c>
-      <c r="I31">
+      <c r="O31">
+        <v>4.2646999999999997E-2</v>
+      </c>
+      <c r="P31">
         <v>-1.0539000000000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q31">
+        <v>8.6843000000000004E-2</v>
+      </c>
+      <c r="R31">
+        <v>-0.39345999999999998</v>
+      </c>
+      <c r="S31">
+        <v>0.33851999999999999</v>
+      </c>
+      <c r="T31">
+        <v>-1.4129</v>
+      </c>
+      <c r="U31">
+        <v>0.35844999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B32">
         <v>0.12153</v>
       </c>
       <c r="C32">
+        <v>0.31163000000000002</v>
+      </c>
+      <c r="D32">
         <v>-0.58450000000000002</v>
       </c>
-      <c r="D32">
+      <c r="E32">
+        <v>0.23966999999999999</v>
+      </c>
+      <c r="F32">
         <v>0.39304</v>
       </c>
-      <c r="E32">
+      <c r="G32">
+        <v>0.43002000000000001</v>
+      </c>
+      <c r="H32">
         <v>-1.1584000000000001</v>
       </c>
-      <c r="F32">
+      <c r="I32">
+        <v>0.38069999999999998</v>
+      </c>
+      <c r="J32">
         <v>0.80735000000000001</v>
       </c>
-      <c r="G32">
+      <c r="K32">
+        <v>0.34505000000000002</v>
+      </c>
+      <c r="L32">
         <v>-0.68615999999999999</v>
       </c>
-      <c r="H32">
+      <c r="M32">
+        <v>0.40794999999999998</v>
+      </c>
+      <c r="N32">
         <v>1.1556999999999999</v>
       </c>
-      <c r="I32">
+      <c r="O32">
+        <v>0.34760999999999997</v>
+      </c>
+      <c r="P32">
         <v>-0.47838000000000003</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q32">
+        <v>0.34227999999999997</v>
+      </c>
+      <c r="R32">
+        <v>0.61939999999999995</v>
+      </c>
+      <c r="S32">
+        <v>0.45535999999999999</v>
+      </c>
+      <c r="T32">
+        <v>-0.72685999999999995</v>
+      </c>
+      <c r="U32">
+        <v>0.29993999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B33">
         <v>-2.2179000000000002</v>
       </c>
       <c r="C33">
+        <v>0.52046000000000003</v>
+      </c>
+      <c r="D33">
         <v>-2.9647000000000001</v>
       </c>
-      <c r="D33">
+      <c r="E33">
+        <v>0.36675000000000002</v>
+      </c>
+      <c r="F33">
         <v>-2.4544000000000001</v>
       </c>
-      <c r="E33">
+      <c r="G33">
+        <v>0.29881000000000002</v>
+      </c>
+      <c r="H33">
         <v>-3.2873999999999999</v>
       </c>
-      <c r="F33">
+      <c r="I33">
+        <v>0.42348999999999998</v>
+      </c>
+      <c r="J33">
         <v>-2.4457</v>
       </c>
-      <c r="G33">
+      <c r="K33">
+        <v>0.42576999999999998</v>
+      </c>
+      <c r="L33">
         <v>-2.1715</v>
       </c>
-      <c r="H33">
+      <c r="M33">
+        <v>0.51849000000000001</v>
+      </c>
+      <c r="N33">
         <v>-2.181</v>
       </c>
-      <c r="I33">
+      <c r="O33">
+        <v>1.0911</v>
+      </c>
+      <c r="P33">
         <v>-2.6726999999999999</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q33">
+        <v>0.53603000000000001</v>
+      </c>
+      <c r="R33">
+        <v>-2.3247</v>
+      </c>
+      <c r="S33">
+        <v>0.14551</v>
+      </c>
+      <c r="T33">
+        <v>-2.7740999999999998</v>
+      </c>
+      <c r="U33">
+        <v>0.47371000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B34">
         <v>-1.5844</v>
       </c>
       <c r="C34">
+        <v>5.4725000000000003E-2</v>
+      </c>
+      <c r="D34">
         <v>0.25464999999999999</v>
       </c>
-      <c r="D34">
+      <c r="E34">
+        <v>0.21958</v>
+      </c>
+      <c r="F34">
         <v>-1.6204000000000001</v>
       </c>
-      <c r="E34">
+      <c r="G34">
+        <v>0.10525</v>
+      </c>
+      <c r="H34">
         <v>8.8054999999999994E-2</v>
       </c>
-      <c r="F34">
+      <c r="I34">
+        <v>0.17896000000000001</v>
+      </c>
+      <c r="J34">
         <v>-1.7607999999999999</v>
       </c>
-      <c r="G34">
+      <c r="K34">
+        <v>0.12826000000000001</v>
+      </c>
+      <c r="L34">
         <v>6.1490999999999997E-2</v>
       </c>
-      <c r="H34">
+      <c r="M34">
+        <v>0.13963999999999999</v>
+      </c>
+      <c r="N34">
         <v>-1.2282999999999999</v>
       </c>
-      <c r="I34">
+      <c r="O34">
+        <v>0.12077</v>
+      </c>
+      <c r="P34">
         <v>0.2311</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q34">
+        <v>0.12501000000000001</v>
+      </c>
+      <c r="R34">
+        <v>-1.5485</v>
+      </c>
+      <c r="S34">
+        <v>0.22661000000000001</v>
+      </c>
+      <c r="T34">
+        <v>0.15881999999999999</v>
+      </c>
+      <c r="U34">
+        <v>9.8129999999999995E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B35">
         <v>-2.0356999999999998</v>
       </c>
       <c r="C35">
+        <v>0.17480000000000001</v>
+      </c>
+      <c r="D35">
         <v>-3.5920999999999998</v>
       </c>
-      <c r="D35">
+      <c r="E35">
+        <v>0.69369000000000003</v>
+      </c>
+      <c r="F35">
         <v>-1.9638</v>
       </c>
-      <c r="E35">
+      <c r="G35">
+        <v>0.25406000000000001</v>
+      </c>
+      <c r="H35">
         <v>-3.6206</v>
       </c>
-      <c r="F35">
+      <c r="I35">
+        <v>0.50954999999999995</v>
+      </c>
+      <c r="J35">
         <v>-1.8946000000000001</v>
       </c>
-      <c r="G35">
+      <c r="K35">
+        <v>0.22850999999999999</v>
+      </c>
+      <c r="L35">
         <v>-3.3117999999999999</v>
       </c>
-      <c r="H35">
+      <c r="M35">
+        <v>0.88536000000000004</v>
+      </c>
+      <c r="N35">
         <v>-1.6584000000000001</v>
       </c>
-      <c r="I35">
+      <c r="O35">
+        <v>0.20468</v>
+      </c>
+      <c r="P35">
         <v>-3.0175999999999998</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q35">
+        <v>0.28025</v>
+      </c>
+      <c r="R35">
+        <v>-1.8880999999999999</v>
+      </c>
+      <c r="S35">
+        <v>0.16363</v>
+      </c>
+      <c r="T35">
+        <v>-3.3855</v>
+      </c>
+      <c r="U35">
+        <v>0.28210000000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B36">
         <v>-0.80405000000000004</v>
       </c>
       <c r="C36">
+        <v>0.34394999999999998</v>
+      </c>
+      <c r="D36">
         <v>-2.9386999999999999</v>
       </c>
-      <c r="D36">
+      <c r="E36">
+        <v>0.46805999999999998</v>
+      </c>
+      <c r="F36">
         <v>0.75273999999999996</v>
       </c>
-      <c r="E36">
+      <c r="G36">
+        <v>0.36659000000000003</v>
+      </c>
+      <c r="H36">
         <v>-3.5476000000000001</v>
       </c>
-      <c r="F36">
+      <c r="I36">
+        <v>0.65522000000000002</v>
+      </c>
+      <c r="J36">
         <v>0.78908</v>
       </c>
-      <c r="G36">
+      <c r="K36">
+        <v>0.27981</v>
+      </c>
+      <c r="L36">
         <v>-2.9860000000000002</v>
       </c>
-      <c r="H36">
+      <c r="M36">
+        <v>0.71296999999999999</v>
+      </c>
+      <c r="N36">
         <v>3.0672999999999999</v>
       </c>
-      <c r="I36">
+      <c r="O36">
+        <v>0.77580000000000005</v>
+      </c>
+      <c r="P36">
         <v>-4.8158000000000003</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q36">
+        <v>1.7616000000000001</v>
+      </c>
+      <c r="R36">
+        <v>0.95126999999999995</v>
+      </c>
+      <c r="S36">
+        <v>1.5942000000000001</v>
+      </c>
+      <c r="T36">
+        <v>-3.5720000000000001</v>
+      </c>
+      <c r="U36">
+        <v>0.87409000000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B37">
         <v>-1.4583999999999999</v>
       </c>
       <c r="C37">
+        <v>0.12257999999999999</v>
+      </c>
+      <c r="D37">
         <v>0.90388999999999997</v>
       </c>
-      <c r="D37">
+      <c r="E37">
+        <v>0.14380000000000001</v>
+      </c>
+      <c r="F37">
         <v>-1.2968</v>
       </c>
-      <c r="E37">
+      <c r="G37">
+        <v>0.21542</v>
+      </c>
+      <c r="H37">
         <v>0.42703000000000002</v>
       </c>
-      <c r="F37">
+      <c r="I37">
+        <v>0.10624</v>
+      </c>
+      <c r="J37">
         <v>-1.7178</v>
       </c>
-      <c r="G37">
+      <c r="K37">
+        <v>0.19184999999999999</v>
+      </c>
+      <c r="L37">
         <v>0.62729000000000001</v>
       </c>
-      <c r="H37">
+      <c r="M37">
+        <v>0.12076000000000001</v>
+      </c>
+      <c r="N37">
         <v>-2.0565000000000002</v>
       </c>
-      <c r="I37">
+      <c r="O37">
+        <v>8.5674E-2</v>
+      </c>
+      <c r="P37">
         <v>0.72582000000000002</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q37">
+        <v>0.11865000000000001</v>
+      </c>
+      <c r="R37">
+        <v>-1.6324000000000001</v>
+      </c>
+      <c r="S37">
+        <v>0.33168999999999998</v>
+      </c>
+      <c r="T37">
+        <v>0.67101</v>
+      </c>
+      <c r="U37">
+        <v>0.19889000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="B38">
         <v>-1.0689</v>
       </c>
       <c r="C38">
+        <v>0.25556000000000001</v>
+      </c>
+      <c r="D38">
         <v>-1.8895999999999999</v>
       </c>
-      <c r="D38">
+      <c r="E38">
+        <v>0.41866999999999999</v>
+      </c>
+      <c r="F38">
         <v>-0.20848</v>
       </c>
-      <c r="E38">
+      <c r="G38">
+        <v>0.20455000000000001</v>
+      </c>
+      <c r="H38">
         <v>-2.0891000000000002</v>
       </c>
-      <c r="F38">
+      <c r="I38">
+        <v>0.63419000000000003</v>
+      </c>
+      <c r="J38">
         <v>0.219</v>
       </c>
-      <c r="G38">
+      <c r="K38">
+        <v>0.20083999999999999</v>
+      </c>
+      <c r="L38">
         <v>-1.7188000000000001</v>
       </c>
-      <c r="H38">
+      <c r="M38">
+        <v>0.36767</v>
+      </c>
+      <c r="N38">
         <v>0.26243</v>
       </c>
-      <c r="I38">
+      <c r="O38">
+        <v>0.23981</v>
+      </c>
+      <c r="P38">
         <v>-0.82172999999999996</v>
+      </c>
+      <c r="Q38">
+        <v>0.64863000000000004</v>
+      </c>
+      <c r="R38">
+        <v>-0.19899</v>
+      </c>
+      <c r="S38">
+        <v>0.61765000000000003</v>
+      </c>
+      <c r="T38">
+        <v>-1.6297999999999999</v>
+      </c>
+      <c r="U38">
+        <v>0.55957000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>